<commit_message>
Started to add year to Size: a size is only for a given year. Some cosmetic improvements: links are bigger. Reimporting doesn't create duplicates anymore.
</commit_message>
<xml_diff>
--- a/doc/data entry.xlsx
+++ b/doc/data entry.xlsx
@@ -11,13 +11,14 @@
     <sheet name="Voile" sheetId="1" r:id="rId2"/>
     <sheet name="Flotteur" sheetId="2" r:id="rId3"/>
     <sheet name="Mat" sheetId="3" r:id="rId4"/>
+    <sheet name="Gaastra" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="47">
   <si>
     <t>Surface</t>
   </si>
@@ -113,6 +114,51 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Kg</t>
+  </si>
+  <si>
+    <t>IMCS</t>
+  </si>
+  <si>
+    <t>Luff</t>
+  </si>
+  <si>
+    <t>Boom</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Batten</t>
+  </si>
+  <si>
+    <t>Head</t>
+  </si>
+  <si>
+    <t>Cams</t>
+  </si>
+  <si>
+    <t>Ideal Mast</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Gaastra 75 RDM</t>
+  </si>
+  <si>
+    <t>Gaastra 75 (75 RDM)</t>
+  </si>
+  <si>
+    <t>Compatible with</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -162,13 +208,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -467,7 +516,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -480,7 +529,7 @@
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1472,4 +1521,304 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:11" ht="30">
+      <c r="A1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30">
+      <c r="A2" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="C2" s="2">
+        <v>400</v>
+      </c>
+      <c r="D2" s="2">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2">
+        <v>406</v>
+      </c>
+      <c r="F2" s="2">
+        <v>168</v>
+      </c>
+      <c r="G2" s="2">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30">
+      <c r="A3" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>400</v>
+      </c>
+      <c r="D3" s="2">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2">
+        <v>423</v>
+      </c>
+      <c r="F3" s="2">
+        <v>172</v>
+      </c>
+      <c r="G3" s="2">
+        <v>23</v>
+      </c>
+      <c r="H3" s="2">
+        <v>6</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30">
+      <c r="A4" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2">
+        <v>430</v>
+      </c>
+      <c r="D4" s="2">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2">
+        <v>439</v>
+      </c>
+      <c r="F4" s="2">
+        <v>178</v>
+      </c>
+      <c r="G4" s="2">
+        <v>9</v>
+      </c>
+      <c r="H4" s="2">
+        <v>6</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30">
+      <c r="A5" s="2">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>430</v>
+      </c>
+      <c r="D5" s="2">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2">
+        <v>450</v>
+      </c>
+      <c r="F5" s="2">
+        <v>185</v>
+      </c>
+      <c r="G5" s="2">
+        <v>20</v>
+      </c>
+      <c r="H5" s="2">
+        <v>6</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="30">
+      <c r="A6" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C6" s="2">
+        <v>430</v>
+      </c>
+      <c r="D6" s="2">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2">
+        <v>453</v>
+      </c>
+      <c r="F6" s="2">
+        <v>198</v>
+      </c>
+      <c r="G6" s="2">
+        <v>23</v>
+      </c>
+      <c r="H6" s="2">
+        <v>6</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="45">
+      <c r="A7" s="2">
+        <v>6.9</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C7" s="2">
+        <v>460</v>
+      </c>
+      <c r="D7" s="2">
+        <v>25</v>
+      </c>
+      <c r="E7" s="2">
+        <v>468</v>
+      </c>
+      <c r="F7" s="2">
+        <v>206</v>
+      </c>
+      <c r="G7" s="2">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2">
+        <v>6</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="45">
+      <c r="A8" s="2">
+        <v>7.4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C8" s="2">
+        <v>460</v>
+      </c>
+      <c r="D8" s="2">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2">
+        <v>478</v>
+      </c>
+      <c r="F8" s="2">
+        <v>218</v>
+      </c>
+      <c r="G8" s="2">
+        <v>18</v>
+      </c>
+      <c r="H8" s="2">
+        <v>6</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30">
+      <c r="A9" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>